<commit_message>
column cleaning for fticr_pores
1. added the sample meta data file
2. this file has all the sample codes. only sample_type "sample" and "as" are actual samples.
3. create a txt file with a list of samples that need to be removed
4. use that file to remove the unnecessary columns
5. three columns (3use, C13, Error_ppm) cannot be removed by that code, so remove them separately.
We now have a file with clean column names.
</commit_message>
<xml_diff>
--- a/data/FTICR_INPUT_SOILPORE_meta.xlsx
+++ b/data/FTICR_INPUT_SOILPORE_meta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pate212/OneDrive - PNNL/Documents/GitHub/3soils_kp/tes_3soils_2019/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_329AAD0241DD5D71D11C342AD980D000A17E3DF4" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{6B48C232-16F3-514A-A906-7B76E042D03F}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_329AAD0241DD5D71D11C342AD980D000A17E3DF4" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{E21FAB88-3D28-7247-AA95-05EAB55C1C3C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1954,13 +1954,13 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A169" sqref="A169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="12" width="8" customWidth="1"/>
     <col min="13" max="26" width="7.6640625" customWidth="1"/>

</xml_diff>